<commit_message>
Implemented: Boost HK3 for autoThreshold OG1 and manual BoostEgK
- WebServer display for testing
</commit_message>
<xml_diff>
--- a/doc/CAN_001_001_01.xlsx
+++ b/doc/CAN_001_001_01.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\dev\knx\EibPC\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\users\asc\repo\EibPC\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C69067D-DFF2-4234-86C3-7743F73DECE0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAN_BC" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="163">
   <si>
     <t>CAN-Eingang(CAN-BC)</t>
   </si>
@@ -75,21 +76,12 @@
     <t>dig.NW.Eing.(UVR1611)</t>
   </si>
   <si>
-    <t>Ref.T.HK2</t>
-  </si>
-  <si>
     <t>Ref.T.HK1</t>
   </si>
   <si>
-    <t>Ref:T:HK4</t>
-  </si>
-  <si>
     <t>Ex.Sw.HK1</t>
   </si>
   <si>
-    <t>Ex.Sw.HK2</t>
-  </si>
-  <si>
     <t>Ex.Sw.HK3</t>
   </si>
   <si>
@@ -213,9 +205,6 @@
     <t>Heat On 9</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>11/3/5</t>
   </si>
   <si>
@@ -480,9 +469,6 @@
     <t>nil</t>
   </si>
   <si>
-    <t>EssZ ZAS</t>
-  </si>
-  <si>
     <t>11/1/4</t>
   </si>
   <si>
@@ -507,12 +493,6 @@
     <t>Boost sw</t>
   </si>
   <si>
-    <t>Sentido Küche mix</t>
-  </si>
-  <si>
-    <t>Ex.Sw.HK5</t>
-  </si>
-  <si>
     <t xml:space="preserve">dep on Valve pos </t>
   </si>
   <si>
@@ -528,22 +508,22 @@
     <t>T.SollHk5</t>
   </si>
   <si>
-    <t>old 6/1/1</t>
-  </si>
-  <si>
     <t>11/3/1</t>
   </si>
   <si>
-    <t>Avg Dach</t>
-  </si>
-  <si>
     <t>Not Used!</t>
+  </si>
+  <si>
+    <t>11/3/2</t>
+  </si>
+  <si>
+    <t>Ref.T.HK4,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -707,7 +687,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -984,51 +964,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C44" workbookViewId="0">
-      <selection activeCell="I64" sqref="I64"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="22.5703125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" style="1"/>
+    <col min="3" max="3" width="22.54296875" style="12" customWidth="1"/>
     <col min="4" max="4" width="16" style="13" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="13" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="23"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="33.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" style="23"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1"/>
+    <col min="8" max="8" width="33.26953125" customWidth="1"/>
+    <col min="9" max="9" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="20"/>
     </row>
-    <row r="2" spans="1:9" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="21"/>
     </row>
-    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="10" t="s">
@@ -1047,10 +1027,10 @@
         <v>6</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C4" s="12">
         <v>1</v>
       </c>
@@ -1061,215 +1041,215 @@
         <v>1</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C5" s="12">
         <v>2</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C6" s="12">
         <v>3</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C7" s="12">
         <v>4</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C8" s="12">
         <v>5</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C9" s="12">
         <v>6</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C10" s="12">
         <v>7</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G10" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C11" s="12">
         <v>8</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G11" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H11" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C12" s="12">
         <v>9</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G12" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C13" s="12">
         <v>10</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G13" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C14" s="12">
         <v>11</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G14" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C15" s="12">
         <v>12</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G15" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C16" s="12">
         <v>13</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G16" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="H16" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="I16" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C17" s="12">
         <v>14</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G17" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H17" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C18" s="12">
         <v>15</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G18" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H18" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C19" s="12">
         <v>16</v>
       </c>
@@ -1277,28 +1257,28 @@
         <v>16</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G19" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="21"/>
     </row>
-    <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="10" t="s">
@@ -1308,7 +1288,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F21" s="22" t="s">
         <v>3</v>
@@ -1317,10 +1297,10 @@
         <v>6</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C22" s="12">
         <v>1</v>
       </c>
@@ -1331,13 +1311,13 @@
         <v>1</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C23" s="12">
         <v>2</v>
       </c>
@@ -1348,13 +1328,13 @@
         <v>2</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C24" s="12">
         <v>3</v>
       </c>
@@ -1365,13 +1345,13 @@
         <v>3</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C25" s="12">
         <v>4</v>
       </c>
@@ -1382,13 +1362,13 @@
         <v>4</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C26" s="12">
         <v>5</v>
       </c>
@@ -1399,13 +1379,13 @@
         <v>5</v>
       </c>
       <c r="F26" s="23" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C27" s="12">
         <v>6</v>
       </c>
@@ -1416,13 +1396,13 @@
         <v>6</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C28" s="12">
         <v>7</v>
       </c>
@@ -1433,13 +1413,13 @@
         <v>7</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C29" s="12">
         <v>8</v>
       </c>
@@ -1447,13 +1427,13 @@
         <v>8</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H29" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C30" s="12">
         <v>9</v>
       </c>
@@ -1461,13 +1441,13 @@
         <v>9</v>
       </c>
       <c r="F30" s="23" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C31" s="12">
         <v>10</v>
       </c>
@@ -1475,13 +1455,13 @@
         <v>10</v>
       </c>
       <c r="F31" s="23" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H31" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C32" s="12">
         <v>11</v>
       </c>
@@ -1489,13 +1469,13 @@
         <v>11</v>
       </c>
       <c r="F32" s="23" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H32" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C33" s="12">
         <v>12</v>
       </c>
@@ -1503,37 +1483,37 @@
         <v>12</v>
       </c>
       <c r="F33" s="23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H33" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C34" s="12">
         <v>13</v>
       </c>
       <c r="H34" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C35" s="12">
         <v>14</v>
       </c>
       <c r="H35" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C36" s="12">
         <v>15</v>
       </c>
       <c r="H36" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C37" s="12">
         <v>16</v>
       </c>
@@ -1541,10 +1521,10 @@
         <v>16</v>
       </c>
       <c r="H37" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>10</v>
       </c>
@@ -1554,19 +1534,19 @@
       <c r="E38" s="8"/>
       <c r="F38" s="20"/>
     </row>
-    <row r="39" spans="1:9" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
       <c r="F39" s="21"/>
     </row>
-    <row r="40" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="10" t="s">
@@ -1585,10 +1565,10 @@
         <v>6</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C41" s="12">
         <v>1</v>
       </c>
@@ -1599,19 +1579,13 @@
         <v>1</v>
       </c>
       <c r="F41" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="G41" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="H41" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C42" s="12">
         <v>2</v>
       </c>
@@ -1622,13 +1596,13 @@
         <v>2</v>
       </c>
       <c r="F42" s="23" t="s">
-        <v>61</v>
+        <v>161</v>
       </c>
       <c r="H42" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C43" s="12">
         <v>3</v>
       </c>
@@ -1639,16 +1613,13 @@
         <v>3</v>
       </c>
       <c r="F43" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="G43" t="s">
-        <v>159</v>
+        <v>102</v>
       </c>
       <c r="H43" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C44" s="12">
         <v>4</v>
       </c>
@@ -1659,16 +1630,13 @@
         <v>4</v>
       </c>
       <c r="F44" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="G44" t="s">
-        <v>168</v>
+        <v>103</v>
       </c>
       <c r="H44" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C45" s="12">
         <v>5</v>
       </c>
@@ -1679,13 +1647,13 @@
         <v>5</v>
       </c>
       <c r="F45" s="23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H45" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C46" s="12">
         <v>6</v>
       </c>
@@ -1696,13 +1664,13 @@
         <v>6</v>
       </c>
       <c r="F46" s="23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H46" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C47" s="12">
         <v>7</v>
       </c>
@@ -1713,13 +1681,10 @@
         <v>7</v>
       </c>
       <c r="F47" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="H47" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C48" s="12">
         <v>8</v>
       </c>
@@ -1730,13 +1695,10 @@
         <v>8</v>
       </c>
       <c r="F48" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="H48" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C49" s="12">
         <v>9</v>
       </c>
@@ -1747,13 +1709,10 @@
         <v>9</v>
       </c>
       <c r="F49" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="H49" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C50" s="12">
         <v>10</v>
       </c>
@@ -1764,70 +1723,70 @@
         <v>10</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C51" s="12">
         <v>11</v>
       </c>
       <c r="F51" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C52" s="12">
         <v>12</v>
       </c>
       <c r="F52" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C53" s="12">
         <v>13</v>
       </c>
       <c r="F53" s="23" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C54" s="12">
         <v>14</v>
       </c>
       <c r="F54" s="23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C55" s="12">
         <v>15</v>
       </c>
       <c r="F55" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C56" s="12">
         <v>16</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="4"/>
       <c r="B57" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
       <c r="F57" s="21"/>
     </row>
-    <row r="58" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="10" t="s">
@@ -1846,10 +1805,10 @@
         <v>6</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C59" s="12">
         <v>1</v>
       </c>
@@ -1860,16 +1819,16 @@
         <v>1</v>
       </c>
       <c r="F59" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G59" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H59" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C60" s="12">
         <v>2</v>
       </c>
@@ -1880,16 +1839,16 @@
         <v>2</v>
       </c>
       <c r="F60" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G60" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H60" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C61" s="12">
         <v>3</v>
       </c>
@@ -1900,16 +1859,16 @@
         <v>3</v>
       </c>
       <c r="F61" s="23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G61" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H61" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C62" s="12">
         <v>4</v>
       </c>
@@ -1920,16 +1879,16 @@
         <v>4</v>
       </c>
       <c r="F62" s="23" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H62" t="s">
+        <v>149</v>
+      </c>
+      <c r="I62" t="s">
         <v>154</v>
       </c>
-      <c r="I62" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C63" s="12">
         <v>5</v>
       </c>
@@ -1940,16 +1899,16 @@
         <v>5</v>
       </c>
       <c r="F63" s="23" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="H63" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I63" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C64" s="12">
         <v>6</v>
       </c>
@@ -1960,61 +1919,61 @@
         <v>6</v>
       </c>
       <c r="F64" s="23" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H64" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="I64" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C65" s="12">
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C66" s="12">
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C67" s="12">
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C68" s="12">
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C69" s="12">
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C70" s="12">
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C71" s="12">
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C72" s="12">
         <v>14</v>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C73" s="12">
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C74" s="12">
         <v>16</v>
       </c>
@@ -2026,140 +1985,140 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" style="15" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" customWidth="1"/>
     <col min="4" max="4" width="14" style="15" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="18">
         <v>1</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C2" s="17">
         <v>1</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="18">
         <v>2</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C3" s="17">
         <v>9</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="18">
         <v>3</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C4" s="17">
         <v>3</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="18">
         <v>4</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C5" s="17">
         <v>8</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="18">
         <v>5</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C6" s="17">
         <v>16</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="18">
         <v>6</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="19"/>
       <c r="E7" s="17"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="18">
         <v>7</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C8" s="17">
         <v>7</v>
@@ -2167,12 +2126,12 @@
       <c r="D8" s="19"/>
       <c r="E8" s="17"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="18">
         <v>8</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C9" s="17">
         <v>11</v>
@@ -2180,12 +2139,12 @@
       <c r="D9" s="19"/>
       <c r="E9" s="17"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="18">
         <v>9</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C10" s="17">
         <v>5</v>
@@ -2193,12 +2152,12 @@
       <c r="D10" s="19"/>
       <c r="E10" s="17"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="18">
         <v>10</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C11" s="17">
         <v>13</v>
@@ -2206,12 +2165,12 @@
       <c r="D11" s="19"/>
       <c r="E11" s="17"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="18">
         <v>11</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C12" s="17">
         <v>4</v>
@@ -2219,12 +2178,12 @@
       <c r="D12" s="19"/>
       <c r="E12" s="17"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="18">
         <v>12</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C13" s="17">
         <v>14</v>
@@ -2232,54 +2191,54 @@
       <c r="D13" s="19"/>
       <c r="E13" s="17"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="18">
         <v>13</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="17"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="18">
         <v>14</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="17"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="18">
         <v>15</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="17"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="18">
         <v>16</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="17"/>

</xml_diff>